<commit_message>
Added flow charts and uml class diagram
</commit_message>
<xml_diff>
--- a/WS325427 Testing Documentation.xlsx
+++ b/WS325427 Testing Documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh_\OneDrive\9DecSoftwareHandIn\WS325427Dec9SoftwareAssessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh_\OneDrive\9DecSoftwareHandIn\WS325427Dec9SoftwareAssessment\SoftwareHandInDecember9Cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2403C5-55B3-4D3F-9F0B-9E3171BAD09B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E42E67D-90BC-4679-ADAE-E5019C56ACD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="1485" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20175" yWindow="6195" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,7 +404,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -601,18 +601,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -762,14 +762,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A758635-5E00-4B74-AE4C-3084238FDC92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{302A89C3-D549-4831-AADD-0C3049F6FC53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -781,6 +773,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A758635-5E00-4B74-AE4C-3084238FDC92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Outputing Costs of Employed Staff
</commit_message>
<xml_diff>
--- a/WS325427 Testing Documentation.xlsx
+++ b/WS325427 Testing Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh_\OneDrive\9DecSoftwareHandIn\WS325427Dec9SoftwareAssessment\SoftwareHandInDecember9Cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D92059-FC5A-44E3-A3F9-DFD64F7B0FBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A571F28A-99DE-43F9-A968-7565160BA794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36975" yWindow="5250" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Test No.</t>
   </si>
@@ -103,6 +103,78 @@
   </si>
   <si>
     <t>Changed condition to while (getline(employeeData, sEmployeeId, ',')) to ensure it doesn’t run by an empty ID and repeat the previous loop</t>
+  </si>
+  <si>
+    <t>3a</t>
+  </si>
+  <si>
+    <t>TestingBreakdown Page</t>
+  </si>
+  <si>
+    <t>Expected to output Job Grades</t>
+  </si>
+  <si>
+    <t>No Outputs</t>
+  </si>
+  <si>
+    <t>cout &lt;&lt; vClsSalariedEmployees[iSalariedEmployeeCount].getJobGrade();</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>sDpeartment and sjobGrade are mixed up</t>
+  </si>
+  <si>
+    <t>3c</t>
+  </si>
+  <si>
+    <t>Outputting Grades</t>
+  </si>
+  <si>
+    <t>Constructors had the wrong ordering of expected arguments, sDepartment and sJobGrade were the other way around with the order of the csv headers</t>
+  </si>
+  <si>
+    <t>Testing Total Amount for salaried staff</t>
+  </si>
+  <si>
+    <t>Total for last person only</t>
+  </si>
+  <si>
+    <t>Loop starting at the end of the vector or maybe only the last guy is being saved when filtering into child classes</t>
+  </si>
+  <si>
+    <t>4a</t>
+  </si>
+  <si>
+    <t>Total for all salaried staff</t>
+  </si>
+  <si>
+    <t>4b</t>
+  </si>
+  <si>
+    <t>Just forgot to add counter to increase index when allocating data so first one was always being overwritten</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>Salaried Staff not finding the hours per week and weeks per year causing wrong calculation of pay</t>
+  </si>
+  <si>
+    <t>Testing Total amount for contracted staff</t>
+  </si>
+  <si>
+    <t>Total of contracted wages</t>
+  </si>
+  <si>
+    <t>Total = 0</t>
+  </si>
+  <si>
+    <t>5b</t>
+  </si>
+  <si>
+    <t>Child Object property was overwriting the parent object method for setting hours and week, removed it to fix this issue</t>
   </si>
 </sst>
 </file>
@@ -173,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -191,6 +263,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -221,9 +299,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3755077</xdr:colOff>
+      <xdr:colOff>3751267</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1351280</xdr:rowOff>
+      <xdr:rowOff>1355090</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -265,9 +343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3370857</xdr:colOff>
+      <xdr:colOff>3374667</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2571749</xdr:rowOff>
+      <xdr:rowOff>2575559</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -309,9 +387,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3183255</xdr:colOff>
+      <xdr:colOff>3179445</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>3255401</xdr:rowOff>
+      <xdr:rowOff>3259211</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -353,9 +431,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5883346</xdr:colOff>
+      <xdr:colOff>5887156</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1392554</xdr:rowOff>
+      <xdr:rowOff>1388744</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -397,7 +475,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6111875</xdr:colOff>
+      <xdr:colOff>6115685</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1030066</xdr:rowOff>
     </xdr:to>
@@ -441,9 +519,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4670194</xdr:colOff>
+      <xdr:colOff>4666384</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>3987550</xdr:rowOff>
+      <xdr:rowOff>3983740</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -468,6 +546,446 @@
         <a:xfrm>
           <a:off x="8888038" y="9684672"/>
           <a:ext cx="4446962" cy="2827233"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>67367</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>73083</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3944505</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1693372</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28C0A30-B765-4E80-8CFA-BBBBE02E6BB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8726458" y="12715356"/>
+          <a:ext cx="3873328" cy="1624099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2074373</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1579765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6492413</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3751095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2099D9D8-BB76-4E64-B259-554A66E7765E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8603328" y="14222038"/>
+          <a:ext cx="6550081" cy="2190380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>121228</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5507182</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1506575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69377EA0-A7D7-44BE-8818-5C7BEF539E48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8780319" y="16729364"/>
+          <a:ext cx="5389764" cy="1337203"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>69274</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>917864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6130638</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1465164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E48E5917-9DFB-4EF1-87BB-C0943F2BA00F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8728365" y="19327091"/>
+          <a:ext cx="6061364" cy="560635"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>34636</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>103910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6682740</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>593437</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50675CF1-97EF-4E90-9120-00C8D0502BA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8693727" y="18513137"/>
+          <a:ext cx="6636674" cy="485717"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9698</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>238644</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7870248</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1180347</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFF9A9FB-CD16-47A5-8910-F46340363680}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8668789" y="20171871"/>
+          <a:ext cx="7870075" cy="941703"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>450274</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>138546</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4435361</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2459134</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B0E1E2-8EAB-49F5-AE56-0F9417C62C1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9109365" y="21457228"/>
+          <a:ext cx="3979372" cy="2314873"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>125037</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>157769</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5963133</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>515865</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAF0B364-287C-4670-8F78-9ABB32EF03C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8784128" y="24056860"/>
+          <a:ext cx="5828571" cy="348571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>46238</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2072294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4497667</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1576617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{833A2DFB-06B5-4C19-98FF-AC97B2D79A43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8705329" y="25971385"/>
+          <a:ext cx="4451429" cy="1617141"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>34636</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1610590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5493684</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>61182</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E736CB12-6AC0-46C0-A424-9C1465D77FE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8693727" y="27622499"/>
+          <a:ext cx="5459048" cy="979047"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -744,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -754,7 +1272,7 @@
     <col min="2" max="2" width="48.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" style="1" customWidth="1"/>
     <col min="4" max="4" width="31.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="93.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="123.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="37.33203125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -851,61 +1369,131 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="146.4" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+    <row r="6" spans="1:6" ht="308.39999999999998" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="146.4" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="120" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="109.2" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="141" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="A9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="202.8" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="166.8" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="A11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="199.8" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="A12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="148.19999999999999" customHeight="1">
       <c r="A13" s="3"/>
@@ -981,18 +1569,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1142,14 +1730,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A758635-5E00-4B74-AE4C-3084238FDC92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{302A89C3-D549-4831-AADD-0C3049F6FC53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1161,6 +1741,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A758635-5E00-4B74-AE4C-3084238FDC92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
addding fixes and versatility to writing csv
</commit_message>
<xml_diff>
--- a/WS325427 Testing Documentation.xlsx
+++ b/WS325427 Testing Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh_\OneDrive\9DecSoftwareHandIn\WS325427Dec9SoftwareAssessment\SoftwareHandInDecember9Cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF9DB0D-3B61-48C0-B8CF-52625CA08046}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF21CDEB-0811-4C4B-B698-772DA0F95437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1307,7 +1307,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1613,18 +1613,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1774,14 +1774,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A758635-5E00-4B74-AE4C-3084238FDC92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{302A89C3-D549-4831-AADD-0C3049F6FC53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1793,6 +1785,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A758635-5E00-4B74-AE4C-3084238FDC92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Bug Fixes and reformatting some functions
</commit_message>
<xml_diff>
--- a/WS325427 Testing Documentation.xlsx
+++ b/WS325427 Testing Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh_\OneDrive\9DecSoftwareHandIn\WS325427Dec9SoftwareAssessment\SoftwareHandInDecember9Cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF21CDEB-0811-4C4B-B698-772DA0F95437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017621AD-C8AE-4666-AA51-A25B730940C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>Test No.</t>
   </si>
@@ -175,6 +175,45 @@
   </si>
   <si>
     <t>Child Object property was overwriting the parent object method for setting hours and week, removed it to fix this issue</t>
+  </si>
+  <si>
+    <t>6a</t>
+  </si>
+  <si>
+    <t>scientific notation is used on large totals</t>
+  </si>
+  <si>
+    <t>raw numbers, 2 decimal places for currency</t>
+  </si>
+  <si>
+    <t>Testing outputs formats of results</t>
+  </si>
+  <si>
+    <t>6b</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Requires formatting using iomanip library std::cout &lt;&lt; std::fixed &lt;&lt; std::setprecision(2)</t>
+  </si>
+  <si>
+    <t>7a</t>
+  </si>
+  <si>
+    <t>Testing Outputs of projects details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exepcted projetc cost to be non zero </t>
+  </si>
+  <si>
+    <t>currently zero</t>
+  </si>
+  <si>
+    <t>there is 1 person assigned to this project in the csv</t>
+  </si>
+  <si>
+    <t>double divided by int was givinga value of 0…</t>
+  </si>
+  <si>
+    <t>7b</t>
   </si>
 </sst>
 </file>
@@ -299,9 +338,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3751267</xdr:colOff>
+      <xdr:colOff>3755077</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1355090</xdr:rowOff>
+      <xdr:rowOff>1351280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -343,9 +382,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3374667</xdr:colOff>
+      <xdr:colOff>3370857</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2575559</xdr:rowOff>
+      <xdr:rowOff>2571749</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -387,9 +426,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3179445</xdr:colOff>
+      <xdr:colOff>3183255</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>3259211</xdr:rowOff>
+      <xdr:rowOff>3255401</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -431,9 +470,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5887156</xdr:colOff>
+      <xdr:colOff>5883346</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1388744</xdr:rowOff>
+      <xdr:rowOff>1392554</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -475,7 +514,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6115685</xdr:colOff>
+      <xdr:colOff>6111875</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1030066</xdr:rowOff>
     </xdr:to>
@@ -519,9 +558,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4666384</xdr:colOff>
+      <xdr:colOff>4670194</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>3983740</xdr:rowOff>
+      <xdr:rowOff>3979930</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -563,9 +602,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3944505</xdr:colOff>
+      <xdr:colOff>3940695</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1693372</xdr:rowOff>
+      <xdr:rowOff>1697182</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -607,9 +646,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6738678</xdr:colOff>
+      <xdr:colOff>6727248</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>3858814</xdr:rowOff>
+      <xdr:rowOff>3868339</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -651,9 +690,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5507182</xdr:colOff>
+      <xdr:colOff>5503372</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>1506575</xdr:rowOff>
+      <xdr:rowOff>1502765</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -697,7 +736,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>6130638</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>1465164</xdr:rowOff>
+      <xdr:rowOff>1468974</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -739,9 +778,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6682740</xdr:colOff>
+      <xdr:colOff>6686550</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>593437</xdr:rowOff>
+      <xdr:rowOff>589627</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -783,7 +822,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7870248</xdr:colOff>
+      <xdr:colOff>7866438</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>1180347</xdr:rowOff>
     </xdr:to>
@@ -827,9 +866,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4435361</xdr:colOff>
+      <xdr:colOff>4439171</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2459134</xdr:rowOff>
+      <xdr:rowOff>2455324</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -871,9 +910,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5963133</xdr:colOff>
+      <xdr:colOff>5959323</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>515865</xdr:rowOff>
+      <xdr:rowOff>512055</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -917,7 +956,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>4497667</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1584236</xdr:rowOff>
+      <xdr:rowOff>1580426</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -959,9 +998,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5497494</xdr:colOff>
+      <xdr:colOff>5507019</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>53563</xdr:rowOff>
+      <xdr:rowOff>57373</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1003,9 +1042,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7827818</xdr:colOff>
+      <xdr:colOff>7831628</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>3629654</xdr:rowOff>
+      <xdr:rowOff>3639179</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1030,6 +1069,226 @@
         <a:xfrm>
           <a:off x="8899640" y="20368089"/>
           <a:ext cx="7587269" cy="1670792"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>640773</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>346364</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6800774</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1660649</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D9C0896-A41A-4323-BD0A-D17F31E65A57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9299864" y="31796182"/>
+          <a:ext cx="6156191" cy="1321905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>658091</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>969819</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7482854</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>2225058</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C09ED85-682F-4804-9AF3-820FB03C6C67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9317182" y="34307319"/>
+          <a:ext cx="6819048" cy="1245714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76893</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>663805</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>8289694</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1925257</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F87DBAF-6EE8-4E8B-B92D-4A1F6A10CF61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8735984" y="37412987"/>
+          <a:ext cx="8218516" cy="1250022"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1943447</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2705447</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4778478</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1333501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CD4CAEA-AA08-4BBE-B9ED-E9190DD880DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10602538" y="39454629"/>
+          <a:ext cx="2835031" cy="1347008"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1437410</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7847041</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>2529489</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27FBBF0B-380D-44C6-930B-9DE8BEE88AE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8857211" y="40905546"/>
+          <a:ext cx="7648921" cy="1092079"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1306,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1540,36 +1799,74 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="148.19999999999999" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="A13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="268.8" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="A14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="214.8" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="A15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="202.2" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="A16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="214.8" customHeight="1">
       <c r="A17" s="3"/>
@@ -1613,18 +1910,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1774,6 +2071,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A758635-5E00-4B74-AE4C-3084238FDC92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{302A89C3-D549-4831-AADD-0C3049F6FC53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1785,14 +2090,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A758635-5E00-4B74-AE4C-3084238FDC92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Error Checking Done. may need additional inputs later
</commit_message>
<xml_diff>
--- a/WS325427 Testing Documentation.xlsx
+++ b/WS325427 Testing Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh_\OneDrive\9DecSoftwareHandIn\WS325427Dec9SoftwareAssessment\SoftwareHandInDecember9Cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017621AD-C8AE-4666-AA51-A25B730940C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82DDFF1-2543-4046-997B-CB3C97FFD031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>Test No.</t>
   </si>
@@ -214,6 +214,30 @@
   </si>
   <si>
     <t>7b</t>
+  </si>
+  <si>
+    <t>Handles the user choice input into one function</t>
+  </si>
+  <si>
+    <t>6 Digits ID Only input and postive only</t>
+  </si>
+  <si>
+    <t>6 digits only</t>
+  </si>
+  <si>
+    <t>Error checks for unwanted user inputs</t>
+  </si>
+  <si>
+    <t>integer inputs are positive and only integer, liekwise for doubles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing no </t>
+  </si>
+  <si>
+    <t>Max of 20 hours, repeats until condition me  tMax of 30weeks, repeats until ocndition met</t>
+  </si>
+  <si>
+    <t>user cant add more hours and weeks than specified</t>
   </si>
 </sst>
 </file>
@@ -284,18 +308,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -338,9 +356,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3755077</xdr:colOff>
+      <xdr:colOff>3751267</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1351280</xdr:rowOff>
+      <xdr:rowOff>1355090</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -382,9 +400,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3370857</xdr:colOff>
+      <xdr:colOff>3374667</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2571749</xdr:rowOff>
+      <xdr:rowOff>2575559</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -426,9 +444,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3183255</xdr:colOff>
+      <xdr:colOff>3179445</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>3255401</xdr:rowOff>
+      <xdr:rowOff>3259211</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -470,9 +488,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5883346</xdr:colOff>
+      <xdr:colOff>5887156</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1392554</xdr:rowOff>
+      <xdr:rowOff>1388744</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -514,7 +532,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6111875</xdr:colOff>
+      <xdr:colOff>6115685</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1030066</xdr:rowOff>
     </xdr:to>
@@ -558,9 +576,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4670194</xdr:colOff>
+      <xdr:colOff>4666384</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>3979930</xdr:rowOff>
+      <xdr:rowOff>3983740</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -602,9 +620,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3940695</xdr:colOff>
+      <xdr:colOff>3944505</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1697182</xdr:rowOff>
+      <xdr:rowOff>1693372</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -646,9 +664,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6727248</xdr:colOff>
+      <xdr:colOff>6723438</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>3868339</xdr:rowOff>
+      <xdr:rowOff>3864529</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -690,9 +708,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5503372</xdr:colOff>
+      <xdr:colOff>5507182</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>1502765</xdr:rowOff>
+      <xdr:rowOff>1506575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -736,7 +754,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>6130638</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>1468974</xdr:rowOff>
+      <xdr:rowOff>1465164</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -778,9 +796,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6686550</xdr:colOff>
+      <xdr:colOff>6682740</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>589627</xdr:rowOff>
+      <xdr:rowOff>593437</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -822,7 +840,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7866438</xdr:colOff>
+      <xdr:colOff>7870248</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>1180347</xdr:rowOff>
     </xdr:to>
@@ -866,9 +884,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4439171</xdr:colOff>
+      <xdr:colOff>4435361</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2455324</xdr:rowOff>
+      <xdr:rowOff>2459134</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -910,9 +928,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5959323</xdr:colOff>
+      <xdr:colOff>5963133</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>512055</xdr:rowOff>
+      <xdr:rowOff>515865</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -956,7 +974,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>4497667</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1580426</xdr:rowOff>
+      <xdr:rowOff>1584236</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -998,9 +1016,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5507019</xdr:colOff>
+      <xdr:colOff>5503209</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>57373</xdr:rowOff>
+      <xdr:rowOff>53563</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1042,9 +1060,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7831628</xdr:colOff>
+      <xdr:colOff>7827818</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>3639179</xdr:rowOff>
+      <xdr:rowOff>3635369</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1086,9 +1104,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6800774</xdr:colOff>
+      <xdr:colOff>6804584</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1660649</xdr:rowOff>
+      <xdr:rowOff>1656839</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1130,9 +1148,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7482854</xdr:colOff>
+      <xdr:colOff>7486664</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2225058</xdr:rowOff>
+      <xdr:rowOff>2228868</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1174,9 +1192,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>8289694</xdr:colOff>
+      <xdr:colOff>8285884</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>1925257</xdr:rowOff>
+      <xdr:rowOff>1921447</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1218,7 +1236,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4778478</xdr:colOff>
+      <xdr:colOff>4782288</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>1333501</xdr:rowOff>
     </xdr:to>
@@ -1264,7 +1282,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>7847041</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>2529489</xdr:rowOff>
+      <xdr:rowOff>2533299</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1289,6 +1307,226 @@
         <a:xfrm>
           <a:off x="8857211" y="40905546"/>
           <a:ext cx="7648921" cy="1092079"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1752946</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>207818</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6019613</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1236388</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D433CDE-D00C-4621-9560-D8002A3FCFDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10412037" y="42256363"/>
+          <a:ext cx="4266667" cy="1041905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1714500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1610590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5889739</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2418209</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5193771-B295-4145-8450-586D6CFEA5A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10373591" y="43659135"/>
+          <a:ext cx="4171429" cy="811429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1802997</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1437409</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6302045</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2305982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5780238D-481F-4D74-ADA3-147227AF9129}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10462088" y="47815500"/>
+          <a:ext cx="4489523" cy="857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2251363</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>294410</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6384696</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>896315</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D4AFC2F-98B0-4360-89E1-D7802A9B2035}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10910454" y="48335046"/>
+          <a:ext cx="4137143" cy="598095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1597083</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>107720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6665653</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>3793433</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52055F9A-5A89-4164-A3CB-382F4BD24D62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10256174" y="49170129"/>
+          <a:ext cx="5068570" cy="3695238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1563,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1601,307 +1839,324 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="209.4" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="298.8" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="128.4" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="324" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="308.39999999999998" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="146.4" customHeight="1">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="349.2" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="109.2" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="202.8" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="166.8" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="5" t="s">
+      <c r="E11" s="5"/>
+      <c r="F11" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="199.8" customHeight="1">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="148.19999999999999" customHeight="1">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="268.8" customHeight="1">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="214.8" customHeight="1">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5" t="s">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="202.2" customHeight="1">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="214.8" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="A17" s="4">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="126.6" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+    <row r="18" spans="1:6" ht="204" customHeight="1">
+      <c r="A18" s="4">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" ht="130.19999999999999" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+    <row r="19" spans="1:6" ht="312.60000000000002" customHeight="1">
+      <c r="A19" s="4">
+        <v>10</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" ht="81" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" ht="105.6" customHeight="1"/>
-    <row r="22" spans="1:6" ht="63" customHeight="1"/>
+    <row r="20" spans="1:6" ht="63" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1910,18 +2165,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2071,14 +2326,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A758635-5E00-4B74-AE4C-3084238FDC92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{302A89C3-D549-4831-AADD-0C3049F6FC53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2090,6 +2337,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A758635-5E00-4B74-AE4C-3084238FDC92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>